<commit_message>
fixed an error in the first sheet
the cell with the title of the column "Point" was empty
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/PLITs/extraction/PLIT_MI.xlsx
+++ b/Multi-taxa_data/PLITs/extraction/PLIT_MI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\COMUNE\STUDIO.LAVORO\IMBRSea\Thesis\StatAnalysis\Multi-taxa_data\PLITs\extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F590180-2D9E-45C3-9FB9-95FB8795A972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BE8E21-D99F-4C2E-AF7E-216BC5D2DDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3905" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3906" uniqueCount="713">
   <si>
     <t>Point</t>
   </si>
@@ -2697,7 +2697,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2770,7 +2770,9 @@
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+      <c r="A4" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -12440,7 +12442,7 @@
   <customSheetViews>
     <customSheetView guid="{0945A032-A38A-4A2D-B08B-EF7107F0CEAA}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A4:L184" xr:uid="{5933FFB7-1173-46B1-B4FA-0BC12E21CA4F}"/>
+      <autoFilter ref="A4:L184" xr:uid="{6477AE4D-A508-4F65-8855-846F24BE7B66}"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="106671713"/>
@@ -22399,7 +22401,9 @@
   </sheetPr>
   <dimension ref="A1:X256"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -26948,7 +26952,7 @@
   <customSheetViews>
     <customSheetView guid="{0945A032-A38A-4A2D-B08B-EF7107F0CEAA}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A4:L229" xr:uid="{E7834E89-5F58-4DBF-88C3-F68D14DEE2BB}"/>
+      <autoFilter ref="A4:L229" xr:uid="{43C3318D-BCE6-4F34-A8E7-AADAFCD3551A}"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="578644007"/>

</xml_diff>